<commit_message>
feat: name of test cases added
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SDET ACADEMY PROJECT\SeleniumMavenFramewoork\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FRAMEWORK_ACADEMY\FrameworkAcademy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFDF458E-E513-46EE-AA24-CA9D99850D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F67BDB5E-0F26-424B-B0CB-84FA68BA3F01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40290" yWindow="2265" windowWidth="18195" windowHeight="13785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -99,7 +99,7 @@
     <t>c22880</t>
   </si>
   <si>
-    <t>jul3ym8odz1</t>
+    <t>juli0o0dz1</t>
   </si>
 </sst>
 </file>
@@ -426,7 +426,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>